<commit_message>
Pushing to updated Github Desktop
No changes
</commit_message>
<xml_diff>
--- a/data/mycobacterium_tuberculosis_mets.xlsx
+++ b/data/mycobacterium_tuberculosis_mets.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\pythonScripts\Mtb_inhibition\Mtb_inhibition\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\pythonScripts\Mtb_inhibition\Mtb_inhibition\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1660C226-0DBA-4863-9B91-672EB10725EC}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAE018EC-FD35-4730-B80A-48032EEF4B83}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5076" activeTab="1" xr2:uid="{F52E7153-7355-4B45-8E7B-A0D46EAB1AA7}"/>
   </bookViews>
@@ -50259,18 +50259,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDA128C9-1410-49B5-94AD-0BC6E9FB384F}">
-  <dimension ref="A1:I1086"/>
+  <dimension ref="A1:L1086"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="30.21875" customWidth="1"/>
+    <col min="2" max="2" width="42.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -50299,7 +50299,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -50327,8 +50327,16 @@
       <c r="I2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K2">
+        <f>COUNTIF(H2:H1086,"=")</f>
+        <v>241</v>
+      </c>
+      <c r="L2">
+        <f>COUNTIF(E2:E1086,"=")</f>
+        <v>293</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -50356,8 +50364,16 @@
       <c r="I3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K3">
+        <f>1085-241</f>
+        <v>844</v>
+      </c>
+      <c r="L3">
+        <f>1085-L2</f>
+        <v>792</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -50386,7 +50402,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -50415,7 +50431,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>37</v>
       </c>
@@ -50444,7 +50460,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>44</v>
       </c>
@@ -50473,7 +50489,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>51</v>
       </c>
@@ -50502,7 +50518,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>58</v>
       </c>
@@ -50531,7 +50547,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>65</v>
       </c>
@@ -50560,7 +50576,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>72</v>
       </c>
@@ -50589,7 +50605,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>79</v>
       </c>
@@ -50618,7 +50634,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>86</v>
       </c>
@@ -50647,7 +50663,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>93</v>
       </c>
@@ -50676,7 +50692,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>100</v>
       </c>
@@ -50705,7 +50721,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>107</v>
       </c>

</xml_diff>